<commit_message>
correct bugs in xlsx/docx file list merging
replaced hand-written code with merge();subset()
</commit_message>
<xml_diff>
--- a/testData/proposalsMixedTest/2023.002A.N.v4.create_subgenus_move_sp_create_sp.xlsx
+++ b/testData/proposalsMixedTest/2023.002A.N.v4.create_subgenus_move_sp_create_sp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtish/Documents/ICTV/validate_proposals/proposalsTest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtish/Documents/ICTV/taxon_proposal_qc_and_load/testData/proposalsMixedTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5926922C-09F4-864A-A9A7-E75F175222A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48103D4B-669D-D744-9F3F-14A6B94CAF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="18560" activeTab="1" xr2:uid="{94A59F7B-7A42-3941-BED7-E7ACB004C4FA}"/>
   </bookViews>
@@ -1251,7 +1251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="124">
   <si>
     <t>Realm</t>
   </si>
@@ -1664,7 +1664,10 @@
     <t>NotBinomial Rhizidiomyces virus</t>
   </si>
   <si>
-    <t>should get error/warning: fails binomial naming</t>
+    <t>should get error/warning: fails binomial naming; no host_source; no accession</t>
+  </si>
+  <si>
+    <t>error: fails biniomial naming</t>
   </si>
 </sst>
 </file>
@@ -2225,9 +2228,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2265,7 +2268,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2371,7 +2374,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2513,7 +2516,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2557,7 +2560,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN7" sqref="AN7"/>
+      <selection pane="bottomLeft" activeCell="AN5" sqref="AN5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2579,7 +2582,7 @@
     <col min="36" max="36" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="12.5" style="4" bestFit="1" customWidth="1"/>
     <col min="38" max="39" width="10.83203125" style="15"/>
-    <col min="40" max="40" width="56.6640625" style="1" customWidth="1"/>
+    <col min="40" max="40" width="67.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.3">
@@ -2910,6 +2913,9 @@
       </c>
       <c r="AM5" s="15" t="s">
         <v>28</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.2">

</xml_diff>